<commit_message>
Gestión de estadísticas funcional
</commit_message>
<xml_diff>
--- a/Resultados Estimación.xlsx
+++ b/Resultados Estimación.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="129">
   <si>
     <t>Código</t>
   </si>
@@ -37,70 +37,270 @@
     <t>Observaciones</t>
   </si>
   <si>
-    <t>Cálculo 1 para Ingeniería</t>
-  </si>
-  <si>
-    <t>Estimación no realizada, asignatura pertenece al módulo básico de ingeniería.</t>
-  </si>
-  <si>
-    <t>Álgebra 1 para Ingeniería</t>
-  </si>
-  <si>
-    <t>Física 1 para Ingeniería</t>
-  </si>
-  <si>
-    <t>Ingeniería y Sustentabilidad</t>
-  </si>
-  <si>
-    <t>Introducción al Diseño en Ingeniería</t>
-  </si>
-  <si>
-    <t>Cálculo 2 para Ingeniería</t>
-  </si>
-  <si>
-    <t>Álgebra 2 para Ingeniería</t>
-  </si>
-  <si>
-    <t>Física 2 para Ingeniería</t>
+    <t>Métodos de programación</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 16, Aprobados Requisito = 17.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 36, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Paradigmas de programación</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 67, Aprobados Requisito = 8.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Análisis de algoritmos y estructura de datos</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 34, Aprobados Requisito = 8.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Fundamentos de ingeniería de software</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 12, Aprobados Requisito = 23.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Algoritmos avanzados</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 5, Aprobados Requisito = 23.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Sistemas operativos</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 41, Aprobados Requisito = 19.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Procesamiento de lenguajes formales</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 17, Aprobados Requisito = 16.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Antropología e ingeniería</t>
+  </si>
+  <si>
+    <t>Estimación no realizada, faltan estadísticas curriculares de los requisitos para estimar esta asignatura.</t>
+  </si>
+  <si>
+    <t>Taller de bases de datos</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 23, Aprobados Requisito = 10.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Redes de computadores</t>
+  </si>
+  <si>
+    <t>Macroeconomía y globalización</t>
+  </si>
+  <si>
+    <t>Estimación no realizada, faltan estadísticas curriculares para estimar esta asignatura.</t>
+  </si>
+  <si>
+    <t>Métodos de ingeniería de software</t>
+  </si>
+  <si>
+    <t>Métodos de optimización</t>
+  </si>
+  <si>
+    <t>Análisis de datos</t>
+  </si>
+  <si>
+    <t>Sistemas de comunicación</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 14, Aprobados Requisito = 17.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Finanzas y contabilidad</t>
+  </si>
+  <si>
+    <t>Estimación no realizada, requisito prioritario pertenece al módulo básico de ingeniería.</t>
+  </si>
+  <si>
+    <t>Administración de proyectos de software</t>
+  </si>
+  <si>
+    <t>Ingeniería y sociedad</t>
+  </si>
+  <si>
+    <t>Modelación y simulación</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 18, Aprobados Requisito = 9.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 32, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Sistemas distribuidos</t>
+  </si>
+  <si>
+    <t>Evaluación de proyectos</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 30, Aprobados Requisito = 17.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Taller de ingeniería de software</t>
+  </si>
+  <si>
+    <t>Tópicos de especialidad 1</t>
+  </si>
+  <si>
+    <t>Tópicos de especialidad 2</t>
+  </si>
+  <si>
+    <t>Tópicos de especialidad 3</t>
+  </si>
+  <si>
+    <t>Seguridad y auditoría informática</t>
+  </si>
+  <si>
+    <t>Proyecto de ingeniería informática</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 8, Aprobados Requisito = 25.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Tópicos de especialidad 4</t>
+  </si>
+  <si>
+    <t>Tópicos de especialidad 5</t>
+  </si>
+  <si>
+    <t>Tópicos de especialidad 6</t>
+  </si>
+  <si>
+    <t>Dirección y gestión de empresas</t>
+  </si>
+  <si>
+    <t>Ingeniería de Sistemas</t>
+  </si>
+  <si>
+    <t>Evaluación y Gestión de Proyectos</t>
+  </si>
+  <si>
+    <t>Informática y Sociedad</t>
+  </si>
+  <si>
+    <t>Sistemas de Información</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 15, Aprobados Requisito = 11.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Técnicas de Ingeniería de Software</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 26, Aprobados Requisito = 10.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Redes computacionales</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 9, Aprobados Requisito = 19.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Proyecto de ingeniería de software</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 18, Aprobados Requisito = 21.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Estructura de computadores</t>
+  </si>
+  <si>
+    <t>Diseño de Bases de Datos</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 15, Aprobados Requisito = 23.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Organización de computadores</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 41, Aprobados Requisito = 6.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 46, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Seminario de computación e informática</t>
+  </si>
+  <si>
+    <t>Trabajo de titulación</t>
+  </si>
+  <si>
+    <t>Diseño de bases de datos</t>
+  </si>
+  <si>
+    <t>Algoritmos Numéricos</t>
+  </si>
+  <si>
+    <t>Inferencia y modelos estadísticos</t>
+  </si>
+  <si>
+    <t>Lógica y teoría de la computación</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 13, Aprobados Requisito = 9.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Seminario de informática</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 10, Aprobados Requisito = 7.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Introducción a Ingeniería Informática</t>
+  </si>
+  <si>
+    <t>Evaluación de Proyectos Informáticos</t>
+  </si>
+  <si>
+    <t>Administración de Proyectos Informáticos</t>
   </si>
   <si>
     <t>Introducción a la Ingeniería Informática</t>
   </si>
   <si>
-    <t>Estimación no realizada, requisito prioritario pertenece al módulo básico de ingeniería.</t>
-  </si>
-  <si>
-    <t>Fundamentos de Programación para Ingeniería</t>
-  </si>
-  <si>
     <t>Fundamentos de Computación</t>
   </si>
   <si>
-    <t>Cálculo y Optimización Multivariable</t>
-  </si>
-  <si>
     <t>Estructura de Datos</t>
   </si>
   <si>
-    <t>Estimación no realizada, faltan estadísticas curriculares de los requisitos para estimar esta asignatura.</t>
-  </si>
-  <si>
-    <t>Electricidad, Magnetismo y Ondas</t>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 49, Aprobados Requisito = 26.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
   </si>
   <si>
     <t>Diseño de Algoritmos</t>
   </si>
   <si>
-    <t>Fundamentos de Economía</t>
-  </si>
-  <si>
-    <t>Inglés 1</t>
-  </si>
-  <si>
-    <t>Ecuaciones Diferenciales y Métodos Numéricos</t>
-  </si>
-  <si>
-    <t>Diseño de Bases de Datos</t>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 39, Aprobados Requisito = 26.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 34, Aprobados Requisito = 26.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
   </si>
   <si>
     <t>Arquitectura de Computadores</t>
@@ -109,10 +309,8 @@
     <t>Paradigmas de Programación</t>
   </si>
   <si>
-    <t>Taller de Diseño en Ingeniería</t>
-  </si>
-  <si>
-    <t>Inglés 2</t>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 26, Aprobados Requisito = 11.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
   </si>
   <si>
     <t>Estadística Computacional</t>
@@ -121,6 +319,10 @@
     <t>Teoría de la Computación</t>
   </si>
   <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 27, Aprobados Requisito = 11.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
     <t>Sistemas Operativos</t>
   </si>
   <si>
@@ -130,27 +332,30 @@
     <t>Taller de Programación</t>
   </si>
   <si>
-    <t>Inglés 3</t>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 10, Aprobados Requisito = 9.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
   </si>
   <si>
     <t>Estadística Inferencial</t>
   </si>
   <si>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 10, Aprobados Requisito = 3.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
+  </si>
+  <si>
     <t>Bases de Datos Avanzadas</t>
   </si>
   <si>
     <t>Procesamiento de Señales e Imágenes</t>
   </si>
   <si>
-    <t>Técnicas de Ingeniería de Software</t>
+    <t>Contribuciones Teoría: Disponibles = 0, Reprobados = 20, Aprobados Requisito = 9.
+Contribuciones Laboratorio: Disponibles = 0, Reprobados = 0, Aprobados Requisito = 0.</t>
   </si>
   <si>
     <t>Evaluación de Proyectos</t>
   </si>
   <si>
-    <t>Inglés 4</t>
-  </si>
-  <si>
     <t>Modelos y Simulación</t>
   </si>
   <si>
@@ -220,187 +425,10 @@
     <t>Trabajo de Titulación</t>
   </si>
   <si>
-    <t>Taller de desarrollo personal e integral</t>
-  </si>
-  <si>
-    <t>Introducción a la Ingeniería</t>
-  </si>
-  <si>
-    <t>Métodos de Estudio</t>
-  </si>
-  <si>
-    <t>Fundamentos de Computación y Programación</t>
-  </si>
-  <si>
-    <t>Química General</t>
-  </si>
-  <si>
-    <t>Introducción a Ingeniería Informática</t>
-  </si>
-  <si>
-    <t>Electricidad y magnetismo para Ingeniería</t>
-  </si>
-  <si>
-    <t>Comunicación efectiva</t>
-  </si>
-  <si>
-    <t>Ecuaciones diferenciales para Ingeniería</t>
-  </si>
-  <si>
-    <t>Métodos de programación</t>
-  </si>
-  <si>
-    <t>Fundamentos de economía</t>
-  </si>
-  <si>
-    <t>Cálculo 3 para Ingeniería</t>
-  </si>
-  <si>
-    <t>Análisis Estadístico para Ingeniería</t>
-  </si>
-  <si>
-    <t>Estructura de computadores</t>
-  </si>
-  <si>
-    <t>Paradigmas de programación</t>
-  </si>
-  <si>
-    <t>Análisis de algoritmos y estructura de datos</t>
-  </si>
-  <si>
-    <t>Ingeniería de Sistemas</t>
-  </si>
-  <si>
-    <t>Diseño de bases de datos</t>
-  </si>
-  <si>
-    <t>Organización de computadores</t>
-  </si>
-  <si>
-    <t>Fundamentos de ingeniería de software</t>
-  </si>
-  <si>
-    <t>Algoritmos avanzados</t>
-  </si>
-  <si>
-    <t>Algoritmos Numéricos</t>
-  </si>
-  <si>
-    <t>Sistemas operativos</t>
-  </si>
-  <si>
-    <t>Procesamiento de lenguajes formales</t>
-  </si>
-  <si>
-    <t>Antropología e ingeniería</t>
-  </si>
-  <si>
-    <t>Taller de bases de datos</t>
-  </si>
-  <si>
-    <t>Inferencia y modelos estadísticos</t>
-  </si>
-  <si>
-    <t>Redes de computadores</t>
-  </si>
-  <si>
-    <t>Lógica y teoría de la computación</t>
-  </si>
-  <si>
-    <t>Macroeconomía y globalización</t>
-  </si>
-  <si>
-    <t>Métodos de ingeniería de software</t>
-  </si>
-  <si>
-    <t>Métodos de optimización</t>
-  </si>
-  <si>
-    <t>Análisis de datos</t>
-  </si>
-  <si>
-    <t>Sistemas de comunicación</t>
-  </si>
-  <si>
-    <t>Finanzas y contabilidad</t>
-  </si>
-  <si>
-    <t>Administración de proyectos de software</t>
-  </si>
-  <si>
-    <t>Ingeniería y sociedad</t>
-  </si>
-  <si>
-    <t>Modelación y simulación</t>
-  </si>
-  <si>
-    <t>Sistemas distribuidos</t>
-  </si>
-  <si>
-    <t>Evaluación de proyectos</t>
-  </si>
-  <si>
-    <t>Taller de ingeniería de software</t>
-  </si>
-  <si>
-    <t>Tópicos de especialidad 1</t>
-  </si>
-  <si>
-    <t>Tópicos de especialidad 2</t>
-  </si>
-  <si>
-    <t>Tópicos de especialidad 3</t>
-  </si>
-  <si>
-    <t>Seguridad y auditoría informática</t>
-  </si>
-  <si>
-    <t>Proyecto de ingeniería informática</t>
-  </si>
-  <si>
-    <t>Tópicos de especialidad 4</t>
-  </si>
-  <si>
-    <t>Tópicos de especialidad 5</t>
-  </si>
-  <si>
-    <t>Tópicos de especialidad 6</t>
-  </si>
-  <si>
-    <t>Dirección y gestión de empresas</t>
-  </si>
-  <si>
-    <t>Seminario de informática</t>
-  </si>
-  <si>
-    <t>Trabajo de titulación</t>
-  </si>
-  <si>
-    <t>Ecuaciones diferenciales y Métodos Numéricos para Ingeniería</t>
-  </si>
-  <si>
-    <t>Evaluación y Gestión de Proyectos</t>
-  </si>
-  <si>
-    <t>Informática y Sociedad</t>
-  </si>
-  <si>
-    <t>Sistemas de Información</t>
-  </si>
-  <si>
-    <t>Evaluación de Proyectos Informáticos</t>
-  </si>
-  <si>
-    <t>Administración de Proyectos Informáticos</t>
-  </si>
-  <si>
-    <t>Redes computacionales</t>
-  </si>
-  <si>
-    <t>Proyecto de ingeniería de software</t>
-  </si>
-  <si>
-    <t>Seminario de computación e informática</t>
+    <t>Calculo 2</t>
+  </si>
+  <si>
+    <t>Estimación no realizada, asignaturas de naturaleza electivos o tópicos no son considerados validos para estimación.</t>
   </si>
 </sst>
 </file>
@@ -773,7 +801,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G135"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -813,22 +841,22 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2">
-        <v>10138</v>
+        <v>13201</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>8</v>
@@ -836,148 +864,148 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2">
-        <v>10139</v>
+        <v>13204</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2">
-        <v>10140</v>
+        <v>13205</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
       <c r="E4" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2">
-        <v>13300</v>
+        <v>13209</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2">
-        <v>10141</v>
+        <v>13210</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2">
-        <v>10142</v>
+        <v>13212</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
       </c>
       <c r="E7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2">
-        <v>10143</v>
+        <v>13213</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2">
-        <v>10144</v>
+        <v>13214</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
@@ -992,38 +1020,38 @@
         <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2">
-        <v>13301</v>
+        <v>13215</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2">
-        <v>10145</v>
+        <v>13217</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2">
         <v>0</v>
@@ -1038,15 +1066,15 @@
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2">
-        <v>13302</v>
+        <v>13219</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -1061,15 +1089,15 @@
         <v>0</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2">
-        <v>13303</v>
+        <v>13220</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2">
         <v>0</v>
@@ -1084,15 +1112,15 @@
         <v>0</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2">
-        <v>13304</v>
+        <v>13221</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2">
         <v>0</v>
@@ -1107,15 +1135,15 @@
         <v>0</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2">
-        <v>13305</v>
+        <v>13222</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2">
         <v>0</v>
@@ -1130,38 +1158,38 @@
         <v>0</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2">
-        <v>13306</v>
+        <v>13223</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
       </c>
       <c r="E16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2">
-        <v>10147</v>
+        <v>13224</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
@@ -1176,15 +1204,15 @@
         <v>0</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2">
-        <v>10130</v>
+        <v>13225</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C18" s="2">
         <v>0</v>
@@ -1199,15 +1227,15 @@
         <v>0</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2">
-        <v>13307</v>
+        <v>13226</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C19" s="2">
         <v>0</v>
@@ -1222,38 +1250,38 @@
         <v>0</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2">
-        <v>13308</v>
+        <v>13227</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C20" s="2">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D20" s="2">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="2">
-        <v>13309</v>
+        <v>13228</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C21" s="2">
         <v>0</v>
@@ -1268,38 +1296,38 @@
         <v>0</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="2">
-        <v>13310</v>
+        <v>13229</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C22" s="2">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
       </c>
       <c r="E22" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22" s="2">
         <v>0</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="2">
-        <v>10148</v>
+        <v>13230</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C23" s="2">
         <v>0</v>
@@ -1314,15 +1342,15 @@
         <v>0</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2">
-        <v>10131</v>
+        <v>13231</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C24" s="2">
         <v>0</v>
@@ -1337,15 +1365,15 @@
         <v>0</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="2">
-        <v>13311</v>
+        <v>13232</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C25" s="2">
         <v>0</v>
@@ -1360,15 +1388,15 @@
         <v>0</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2">
-        <v>13312</v>
+        <v>13233</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C26" s="2">
         <v>0</v>
@@ -1388,10 +1416,10 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="2">
-        <v>13313</v>
+        <v>13234</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C27" s="2">
         <v>0</v>
@@ -1406,38 +1434,38 @@
         <v>0</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2">
-        <v>13314</v>
+        <v>13235</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C28" s="2">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D28" s="2">
         <v>0</v>
       </c>
       <c r="E28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="2">
         <v>0</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2">
-        <v>13315</v>
+        <v>13236</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C29" s="2">
         <v>0</v>
@@ -1457,10 +1485,10 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="2">
-        <v>10132</v>
+        <v>13237</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C30" s="2">
         <v>0</v>
@@ -1475,15 +1503,15 @@
         <v>0</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2">
-        <v>13316</v>
+        <v>13238</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C31" s="2">
         <v>0</v>
@@ -1503,10 +1531,10 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="2">
-        <v>13317</v>
+        <v>13239</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C32" s="2">
         <v>0</v>
@@ -1521,15 +1549,15 @@
         <v>0</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="2">
-        <v>13318</v>
+        <v>13252</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C33" s="2">
         <v>0</v>
@@ -1544,15 +1572,15 @@
         <v>0</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="2">
-        <v>13319</v>
+        <v>13256</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C34" s="2">
         <v>0</v>
@@ -1572,10 +1600,10 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="2">
-        <v>13320</v>
+        <v>13260</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C35" s="2">
         <v>0</v>
@@ -1590,107 +1618,107 @@
         <v>0</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="2">
-        <v>10133</v>
+        <v>13261</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C36" s="2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D36" s="2">
         <v>0</v>
       </c>
       <c r="E36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="2">
         <v>0</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="2">
-        <v>13321</v>
+        <v>13265</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C37" s="2">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D37" s="2">
         <v>0</v>
       </c>
       <c r="E37" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F37" s="2">
         <v>0</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="2">
-        <v>13322</v>
+        <v>13266</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C38" s="2">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D38" s="2">
         <v>0</v>
       </c>
       <c r="E38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="2">
         <v>0</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="2">
-        <v>13323</v>
+        <v>13267</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C39" s="2">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="D39" s="2">
         <v>0</v>
       </c>
       <c r="E39" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F39" s="2">
         <v>0</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="2">
-        <v>13324</v>
+        <v>13268</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C40" s="2">
         <v>0</v>
@@ -1710,10 +1738,10 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="2">
-        <v>13325</v>
+        <v>13269</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C41" s="2">
         <v>0</v>
@@ -1733,10 +1761,10 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="2">
-        <v>13326</v>
+        <v>13270</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C42" s="2">
         <v>0</v>
@@ -1751,15 +1779,15 @@
         <v>0</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="2">
-        <v>13327</v>
+        <v>13273</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C43" s="2">
         <v>0</v>
@@ -1774,84 +1802,84 @@
         <v>0</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="2">
-        <v>13328</v>
+        <v>13274</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C44" s="2">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="D44" s="2">
         <v>0</v>
       </c>
       <c r="E44" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F44" s="2">
         <v>0</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="2">
-        <v>13329</v>
+        <v>13275</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C45" s="2">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="D45" s="2">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E45" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F45" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="2">
-        <v>13330</v>
+        <v>13276</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C46" s="2">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D46" s="2">
         <v>0</v>
       </c>
       <c r="E46" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F46" s="2">
         <v>0</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="2">
-        <v>13331</v>
+        <v>13277</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="C47" s="2">
         <v>0</v>
@@ -1866,15 +1894,15 @@
         <v>0</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="2">
-        <v>13332</v>
+        <v>13278</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C48" s="2">
         <v>0</v>
@@ -1889,15 +1917,15 @@
         <v>0</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="2">
-        <v>13333</v>
+        <v>13279</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C49" s="2">
         <v>0</v>
@@ -1912,15 +1940,15 @@
         <v>0</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="2">
-        <v>13334</v>
+        <v>13280</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C50" s="2">
         <v>0</v>
@@ -1935,15 +1963,15 @@
         <v>0</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="2">
-        <v>13335</v>
+        <v>13281</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C51" s="2">
         <v>0</v>
@@ -1963,10 +1991,10 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="2">
-        <v>13336</v>
+        <v>13282</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C52" s="2">
         <v>0</v>
@@ -1981,15 +2009,15 @@
         <v>0</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="2">
-        <v>13337</v>
+        <v>13283</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C53" s="2">
         <v>0</v>
@@ -2004,61 +2032,61 @@
         <v>0</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="2">
-        <v>13338</v>
+        <v>13284</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="C54" s="2">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D54" s="2">
         <v>0</v>
       </c>
       <c r="E54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54" s="2">
         <v>0</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="2">
-        <v>13339</v>
+        <v>13285</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C55" s="2">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D55" s="2">
         <v>0</v>
       </c>
       <c r="E55" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" s="2">
         <v>0</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="2">
-        <v>13340</v>
+        <v>13286</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C56" s="2">
         <v>0</v>
@@ -2073,15 +2101,15 @@
         <v>0</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="2">
-        <v>13341</v>
+        <v>13287</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C57" s="2">
         <v>0</v>
@@ -2096,15 +2124,15 @@
         <v>0</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="2">
-        <v>13342</v>
+        <v>13288</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C58" s="2">
         <v>0</v>
@@ -2119,15 +2147,15 @@
         <v>0</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="2">
-        <v>13343</v>
+        <v>13289</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C59" s="2">
         <v>0</v>
@@ -2147,10 +2175,10 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="2">
-        <v>10101</v>
+        <v>13301</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="C60" s="2">
         <v>0</v>
@@ -2165,15 +2193,15 @@
         <v>0</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="2">
-        <v>10102</v>
+        <v>13302</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="C61" s="2">
         <v>0</v>
@@ -2188,84 +2216,84 @@
         <v>0</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="2">
-        <v>10103</v>
+        <v>13304</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="C62" s="2">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="D62" s="2">
         <v>0</v>
       </c>
       <c r="E62" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F62" s="2">
         <v>0</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>8</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="2">
-        <v>10104</v>
+        <v>13306</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="C63" s="2">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="D63" s="2">
         <v>0</v>
       </c>
       <c r="E63" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F63" s="2">
         <v>0</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="2">
-        <v>10125</v>
+        <v>13308</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C64" s="2">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="D64" s="2">
         <v>0</v>
       </c>
       <c r="E64" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F64" s="2">
         <v>0</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="2">
-        <v>10126</v>
+        <v>13309</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="C65" s="2">
         <v>0</v>
@@ -2280,38 +2308,38 @@
         <v>0</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="2">
-        <v>10107</v>
+        <v>13310</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="C66" s="2">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="D66" s="2">
         <v>0</v>
       </c>
       <c r="E66" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F66" s="2">
         <v>0</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="2">
-        <v>10108</v>
+        <v>13311</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="C67" s="2">
         <v>0</v>
@@ -2326,38 +2354,38 @@
         <v>0</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="2">
-        <v>10109</v>
+        <v>13312</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="C68" s="2">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="D68" s="2">
         <v>0</v>
       </c>
       <c r="E68" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F68" s="2">
         <v>0</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="2">
-        <v>10110</v>
+        <v>13313</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="C69" s="2">
         <v>0</v>
@@ -2372,15 +2400,15 @@
         <v>0</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="2">
-        <v>10111</v>
+        <v>13314</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="C70" s="2">
         <v>0</v>
@@ -2395,61 +2423,61 @@
         <v>0</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="2">
-        <v>13287</v>
+        <v>13315</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="C71" s="2">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D71" s="2">
         <v>0</v>
       </c>
       <c r="E71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F71" s="2">
         <v>0</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="2">
-        <v>10127</v>
+        <v>13316</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="C72" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D72" s="2">
         <v>0</v>
       </c>
       <c r="E72" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F72" s="2">
         <v>0</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>8</v>
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="2">
-        <v>10128</v>
+        <v>13317</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="C73" s="2">
         <v>0</v>
@@ -2464,38 +2492,38 @@
         <v>0</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="2">
-        <v>10122</v>
+        <v>13318</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="C74" s="2">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D74" s="2">
         <v>0</v>
       </c>
       <c r="E74" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F74" s="2">
         <v>0</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="2">
-        <v>13201</v>
+        <v>13319</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C75" s="2">
         <v>0</v>
@@ -2515,10 +2543,10 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="2">
-        <v>10116</v>
+        <v>13320</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="C76" s="2">
         <v>0</v>
@@ -2533,15 +2561,15 @@
         <v>0</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="2">
-        <v>10129</v>
+        <v>13321</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="C77" s="2">
         <v>0</v>
@@ -2556,15 +2584,15 @@
         <v>0</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="2">
-        <v>10115</v>
+        <v>13322</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="C78" s="2">
         <v>0</v>
@@ -2579,15 +2607,15 @@
         <v>0</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="2">
-        <v>13278</v>
+        <v>13323</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="C79" s="2">
         <v>0</v>
@@ -2602,15 +2630,15 @@
         <v>0</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="2">
-        <v>13204</v>
+        <v>13324</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="C80" s="2">
         <v>0</v>
@@ -2630,10 +2658,10 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="2">
-        <v>13205</v>
+        <v>13325</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C81" s="2">
         <v>0</v>
@@ -2653,10 +2681,10 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="2">
-        <v>13279</v>
+        <v>13326</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="C82" s="2">
         <v>0</v>
@@ -2671,15 +2699,15 @@
         <v>0</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="2">
-        <v>13280</v>
+        <v>13327</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="C83" s="2">
         <v>0</v>
@@ -2699,10 +2727,10 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="2">
-        <v>13281</v>
+        <v>13328</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="C84" s="2">
         <v>0</v>
@@ -2722,10 +2750,10 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="2">
-        <v>13209</v>
+        <v>13329</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="C85" s="2">
         <v>0</v>
@@ -2745,10 +2773,10 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="2">
-        <v>13210</v>
+        <v>13330</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="C86" s="2">
         <v>0</v>
@@ -2768,10 +2796,10 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="2">
-        <v>13282</v>
+        <v>13331</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="C87" s="2">
         <v>0</v>
@@ -2786,15 +2814,15 @@
         <v>0</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="2">
-        <v>13212</v>
+        <v>13332</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="C88" s="2">
         <v>0</v>
@@ -2809,15 +2837,15 @@
         <v>0</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" s="2">
-        <v>13213</v>
+        <v>13333</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="C89" s="2">
         <v>0</v>
@@ -2837,10 +2865,10 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="2">
-        <v>13214</v>
+        <v>13334</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="C90" s="2">
         <v>0</v>
@@ -2860,10 +2888,10 @@
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="2">
-        <v>13215</v>
+        <v>13335</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="C91" s="2">
         <v>0</v>
@@ -2883,10 +2911,10 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="2">
-        <v>13283</v>
+        <v>13336</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="C92" s="2">
         <v>0</v>
@@ -2901,15 +2929,15 @@
         <v>0</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" s="2">
-        <v>13217</v>
+        <v>13337</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="C93" s="2">
         <v>0</v>
@@ -2929,10 +2957,10 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="2">
-        <v>13284</v>
+        <v>13338</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="C94" s="2">
         <v>0</v>
@@ -2952,10 +2980,10 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="2">
-        <v>13219</v>
+        <v>13339</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="C95" s="2">
         <v>0</v>
@@ -2975,10 +3003,10 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="2">
-        <v>13220</v>
+        <v>13340</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="C96" s="2">
         <v>0</v>
@@ -2998,10 +3026,10 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" s="2">
-        <v>13221</v>
+        <v>13341</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="C97" s="2">
         <v>0</v>
@@ -3021,10 +3049,10 @@
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="2">
-        <v>13222</v>
+        <v>13342</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="C98" s="2">
         <v>0</v>
@@ -3044,10 +3072,10 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="2">
-        <v>13223</v>
+        <v>13343</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="C99" s="2">
         <v>0</v>
@@ -3067,10 +3095,10 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100" s="2">
-        <v>13224</v>
+        <v>13999</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="C100" s="2">
         <v>0</v>
@@ -3085,812 +3113,7 @@
         <v>0</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7">
-      <c r="A101" s="2">
-        <v>13225</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C101" s="2">
-        <v>0</v>
-      </c>
-      <c r="D101" s="2">
-        <v>0</v>
-      </c>
-      <c r="E101" s="2">
-        <v>0</v>
-      </c>
-      <c r="F101" s="2">
-        <v>0</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7">
-      <c r="A102" s="2">
-        <v>13226</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C102" s="2">
-        <v>0</v>
-      </c>
-      <c r="D102" s="2">
-        <v>0</v>
-      </c>
-      <c r="E102" s="2">
-        <v>0</v>
-      </c>
-      <c r="F102" s="2">
-        <v>0</v>
-      </c>
-      <c r="G102" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7">
-      <c r="A103" s="2">
-        <v>13227</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C103" s="2">
-        <v>0</v>
-      </c>
-      <c r="D103" s="2">
-        <v>0</v>
-      </c>
-      <c r="E103" s="2">
-        <v>0</v>
-      </c>
-      <c r="F103" s="2">
-        <v>0</v>
-      </c>
-      <c r="G103" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7">
-      <c r="A104" s="2">
-        <v>13228</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C104" s="2">
-        <v>0</v>
-      </c>
-      <c r="D104" s="2">
-        <v>0</v>
-      </c>
-      <c r="E104" s="2">
-        <v>0</v>
-      </c>
-      <c r="F104" s="2">
-        <v>0</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7">
-      <c r="A105" s="2">
-        <v>13229</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C105" s="2">
-        <v>0</v>
-      </c>
-      <c r="D105" s="2">
-        <v>0</v>
-      </c>
-      <c r="E105" s="2">
-        <v>0</v>
-      </c>
-      <c r="F105" s="2">
-        <v>0</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7">
-      <c r="A106" s="2">
-        <v>13230</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C106" s="2">
-        <v>0</v>
-      </c>
-      <c r="D106" s="2">
-        <v>0</v>
-      </c>
-      <c r="E106" s="2">
-        <v>0</v>
-      </c>
-      <c r="F106" s="2">
-        <v>0</v>
-      </c>
-      <c r="G106" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7">
-      <c r="A107" s="2">
-        <v>13231</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C107" s="2">
-        <v>0</v>
-      </c>
-      <c r="D107" s="2">
-        <v>0</v>
-      </c>
-      <c r="E107" s="2">
-        <v>0</v>
-      </c>
-      <c r="F107" s="2">
-        <v>0</v>
-      </c>
-      <c r="G107" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7">
-      <c r="A108" s="2">
-        <v>13232</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C108" s="2">
-        <v>0</v>
-      </c>
-      <c r="D108" s="2">
-        <v>0</v>
-      </c>
-      <c r="E108" s="2">
-        <v>0</v>
-      </c>
-      <c r="F108" s="2">
-        <v>0</v>
-      </c>
-      <c r="G108" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7">
-      <c r="A109" s="2">
-        <v>13233</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C109" s="2">
-        <v>0</v>
-      </c>
-      <c r="D109" s="2">
-        <v>0</v>
-      </c>
-      <c r="E109" s="2">
-        <v>0</v>
-      </c>
-      <c r="F109" s="2">
-        <v>0</v>
-      </c>
-      <c r="G109" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7">
-      <c r="A110" s="2">
-        <v>13234</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C110" s="2">
-        <v>0</v>
-      </c>
-      <c r="D110" s="2">
-        <v>0</v>
-      </c>
-      <c r="E110" s="2">
-        <v>0</v>
-      </c>
-      <c r="F110" s="2">
-        <v>0</v>
-      </c>
-      <c r="G110" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7">
-      <c r="A111" s="2">
-        <v>13235</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C111" s="2">
-        <v>0</v>
-      </c>
-      <c r="D111" s="2">
-        <v>0</v>
-      </c>
-      <c r="E111" s="2">
-        <v>0</v>
-      </c>
-      <c r="F111" s="2">
-        <v>0</v>
-      </c>
-      <c r="G111" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7">
-      <c r="A112" s="2">
-        <v>13236</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C112" s="2">
-        <v>0</v>
-      </c>
-      <c r="D112" s="2">
-        <v>0</v>
-      </c>
-      <c r="E112" s="2">
-        <v>0</v>
-      </c>
-      <c r="F112" s="2">
-        <v>0</v>
-      </c>
-      <c r="G112" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7">
-      <c r="A113" s="2">
-        <v>13237</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C113" s="2">
-        <v>0</v>
-      </c>
-      <c r="D113" s="2">
-        <v>0</v>
-      </c>
-      <c r="E113" s="2">
-        <v>0</v>
-      </c>
-      <c r="F113" s="2">
-        <v>0</v>
-      </c>
-      <c r="G113" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7">
-      <c r="A114" s="2">
-        <v>13238</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C114" s="2">
-        <v>0</v>
-      </c>
-      <c r="D114" s="2">
-        <v>0</v>
-      </c>
-      <c r="E114" s="2">
-        <v>0</v>
-      </c>
-      <c r="F114" s="2">
-        <v>0</v>
-      </c>
-      <c r="G114" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7">
-      <c r="A115" s="2">
-        <v>13239</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C115" s="2">
-        <v>0</v>
-      </c>
-      <c r="D115" s="2">
-        <v>0</v>
-      </c>
-      <c r="E115" s="2">
-        <v>0</v>
-      </c>
-      <c r="F115" s="2">
-        <v>0</v>
-      </c>
-      <c r="G115" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7">
-      <c r="A116" s="2">
-        <v>13285</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C116" s="2">
-        <v>0</v>
-      </c>
-      <c r="D116" s="2">
-        <v>0</v>
-      </c>
-      <c r="E116" s="2">
-        <v>0</v>
-      </c>
-      <c r="F116" s="2">
-        <v>0</v>
-      </c>
-      <c r="G116" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7">
-      <c r="A117" s="2">
-        <v>13286</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C117" s="2">
-        <v>0</v>
-      </c>
-      <c r="D117" s="2">
-        <v>0</v>
-      </c>
-      <c r="E117" s="2">
-        <v>0</v>
-      </c>
-      <c r="F117" s="2">
-        <v>0</v>
-      </c>
-      <c r="G117" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7">
-      <c r="A118" s="2">
-        <v>10123</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C118" s="2">
-        <v>0</v>
-      </c>
-      <c r="D118" s="2">
-        <v>0</v>
-      </c>
-      <c r="E118" s="2">
-        <v>0</v>
-      </c>
-      <c r="F118" s="2">
-        <v>0</v>
-      </c>
-      <c r="G118" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7">
-      <c r="A119" s="2">
-        <v>13252</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C119" s="2">
-        <v>0</v>
-      </c>
-      <c r="D119" s="2">
-        <v>0</v>
-      </c>
-      <c r="E119" s="2">
-        <v>0</v>
-      </c>
-      <c r="F119" s="2">
-        <v>0</v>
-      </c>
-      <c r="G119" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7">
-      <c r="A120" s="2">
-        <v>13273</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C120" s="2">
-        <v>0</v>
-      </c>
-      <c r="D120" s="2">
-        <v>0</v>
-      </c>
-      <c r="E120" s="2">
-        <v>0</v>
-      </c>
-      <c r="F120" s="2">
-        <v>0</v>
-      </c>
-      <c r="G120" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7">
-      <c r="A121" s="2">
-        <v>13256</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C121" s="2">
-        <v>0</v>
-      </c>
-      <c r="D121" s="2">
-        <v>0</v>
-      </c>
-      <c r="E121" s="2">
-        <v>0</v>
-      </c>
-      <c r="F121" s="2">
-        <v>0</v>
-      </c>
-      <c r="G121" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7">
-      <c r="A122" s="2">
-        <v>13260</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C122" s="2">
-        <v>0</v>
-      </c>
-      <c r="D122" s="2">
-        <v>0</v>
-      </c>
-      <c r="E122" s="2">
-        <v>0</v>
-      </c>
-      <c r="F122" s="2">
-        <v>0</v>
-      </c>
-      <c r="G122" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7">
-      <c r="A123" s="2">
-        <v>13261</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C123" s="2">
-        <v>0</v>
-      </c>
-      <c r="D123" s="2">
-        <v>0</v>
-      </c>
-      <c r="E123" s="2">
-        <v>0</v>
-      </c>
-      <c r="F123" s="2">
-        <v>0</v>
-      </c>
-      <c r="G123" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7">
-      <c r="A124" s="2">
-        <v>13274</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C124" s="2">
-        <v>0</v>
-      </c>
-      <c r="D124" s="2">
-        <v>0</v>
-      </c>
-      <c r="E124" s="2">
-        <v>0</v>
-      </c>
-      <c r="F124" s="2">
-        <v>0</v>
-      </c>
-      <c r="G124" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7">
-      <c r="A125" s="2">
-        <v>13275</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C125" s="2">
-        <v>0</v>
-      </c>
-      <c r="D125" s="2">
-        <v>0</v>
-      </c>
-      <c r="E125" s="2">
-        <v>0</v>
-      </c>
-      <c r="F125" s="2">
-        <v>0</v>
-      </c>
-      <c r="G125" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7">
-      <c r="A126" s="2">
-        <v>13288</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C126" s="2">
-        <v>0</v>
-      </c>
-      <c r="D126" s="2">
-        <v>0</v>
-      </c>
-      <c r="E126" s="2">
-        <v>0</v>
-      </c>
-      <c r="F126" s="2">
-        <v>0</v>
-      </c>
-      <c r="G126" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7">
-      <c r="A127" s="2">
-        <v>13289</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C127" s="2">
-        <v>0</v>
-      </c>
-      <c r="D127" s="2">
-        <v>0</v>
-      </c>
-      <c r="E127" s="2">
-        <v>0</v>
-      </c>
-      <c r="F127" s="2">
-        <v>0</v>
-      </c>
-      <c r="G127" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7">
-      <c r="A128" s="2">
-        <v>13265</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C128" s="2">
-        <v>0</v>
-      </c>
-      <c r="D128" s="2">
-        <v>0</v>
-      </c>
-      <c r="E128" s="2">
-        <v>0</v>
-      </c>
-      <c r="F128" s="2">
-        <v>0</v>
-      </c>
-      <c r="G128" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7">
-      <c r="A129" s="2">
-        <v>13266</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C129" s="2">
-        <v>0</v>
-      </c>
-      <c r="D129" s="2">
-        <v>0</v>
-      </c>
-      <c r="E129" s="2">
-        <v>0</v>
-      </c>
-      <c r="F129" s="2">
-        <v>0</v>
-      </c>
-      <c r="G129" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7">
-      <c r="A130" s="2">
-        <v>13267</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C130" s="2">
-        <v>0</v>
-      </c>
-      <c r="D130" s="2">
-        <v>0</v>
-      </c>
-      <c r="E130" s="2">
-        <v>0</v>
-      </c>
-      <c r="F130" s="2">
-        <v>0</v>
-      </c>
-      <c r="G130" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7">
-      <c r="A131" s="2">
-        <v>13268</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C131" s="2">
-        <v>0</v>
-      </c>
-      <c r="D131" s="2">
-        <v>0</v>
-      </c>
-      <c r="E131" s="2">
-        <v>0</v>
-      </c>
-      <c r="F131" s="2">
-        <v>0</v>
-      </c>
-      <c r="G131" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7">
-      <c r="A132" s="2">
-        <v>13269</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C132" s="2">
-        <v>0</v>
-      </c>
-      <c r="D132" s="2">
-        <v>0</v>
-      </c>
-      <c r="E132" s="2">
-        <v>0</v>
-      </c>
-      <c r="F132" s="2">
-        <v>0</v>
-      </c>
-      <c r="G132" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7">
-      <c r="A133" s="2">
-        <v>13270</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C133" s="2">
-        <v>0</v>
-      </c>
-      <c r="D133" s="2">
-        <v>0</v>
-      </c>
-      <c r="E133" s="2">
-        <v>0</v>
-      </c>
-      <c r="F133" s="2">
-        <v>0</v>
-      </c>
-      <c r="G133" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7">
-      <c r="A134" s="2">
-        <v>13276</v>
-      </c>
-      <c r="B134" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="C134" s="2">
-        <v>0</v>
-      </c>
-      <c r="D134" s="2">
-        <v>0</v>
-      </c>
-      <c r="E134" s="2">
-        <v>0</v>
-      </c>
-      <c r="F134" s="2">
-        <v>0</v>
-      </c>
-      <c r="G134" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7">
-      <c r="A135" s="2">
-        <v>13277</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C135" s="2">
-        <v>0</v>
-      </c>
-      <c r="D135" s="2">
-        <v>0</v>
-      </c>
-      <c r="E135" s="2">
-        <v>0</v>
-      </c>
-      <c r="F135" s="2">
-        <v>0</v>
-      </c>
-      <c r="G135" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>